<commit_message>
Page object model practice 2
</commit_message>
<xml_diff>
--- a/ExcelFiles/TutorialsNinja.xlsx
+++ b/ExcelFiles/TutorialsNinja.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ManjiriGosavi\PycharmProjects\SeleniumTutorialsninjaPythonFramework\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE95156E-8008-4017-8741-EE7A7E5B4794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0033CC73-56CD-4F05-B70A-2EE7E1B6370D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTest" sheetId="1" r:id="rId1"/>
+    <sheet name="RegisterTest" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Username</t>
   </si>
@@ -49,6 +50,18 @@
   </si>
   <si>
     <t>Team@1234</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Here</t>
   </si>
 </sst>
 </file>
@@ -135,13 +148,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -425,7 +441,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -478,4 +494,41 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B8218A8-0590-465D-8F8E-C032821A6581}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.36328125" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="12.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="7"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>